<commit_message>
forgot to save sth
</commit_message>
<xml_diff>
--- a/P2/data/rendimiento.xlsx
+++ b/P2/data/rendimiento.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>classclassic</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Turno</t>
+  </si>
+  <si>
+    <t>Segundos</t>
   </si>
 </sst>
 </file>
@@ -158,6 +161,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Fantasmas comidos según la</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t> distancia avanzada por el Agente</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -172,7 +205,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -192,7 +225,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -209,8 +242,10 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2112,7 +2147,7 @@
                   <c:v>625.0</c:v>
                 </c:pt>
                 <c:pt idx="625">
-                  <c:v>656.0</c:v>
+                  <c:v>626.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4004,7 +4039,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4021,8 +4056,10 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -5924,7 +5961,7 @@
                   <c:v>625.0</c:v>
                 </c:pt>
                 <c:pt idx="625">
-                  <c:v>656.0</c:v>
+                  <c:v>626.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7816,7 +7853,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -7833,8 +7870,10 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -9736,7 +9775,7 @@
                   <c:v>625.0</c:v>
                 </c:pt>
                 <c:pt idx="625">
-                  <c:v>656.0</c:v>
+                  <c:v>626.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11628,7 +11667,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -11645,6 +11684,7 @@
         <c:axId val="-2095900112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -11662,6 +11702,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11683,7 +11724,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -11707,6 +11748,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -11724,6 +11766,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11745,7 +11788,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -11790,7 +11833,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -11806,6 +11849,446 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Tiempo medio de respuesta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> del agente (en segundos)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Segundos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00153847842190458"/>
+                  <c:y val="-0.125374589098693"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.82866470960445E-5"/>
+                  <c:y val="-0.431981117651556"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00134544157590057"/>
+                  <c:y val="-0.114609165965905"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$U$42:$W$42</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Práctica 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Práctica 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Teclado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$43:$W$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.00227041549682616</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0827796042911672</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000618845224380375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2052631584"/>
+        <c:axId val="-2095200368"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2052631584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2095200368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2095200368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2052631584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -11880,6 +12363,12 @@
     <a:lumMod val="50000"/>
     <a:lumOff val="50000"/>
   </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
 </cs:colorStyle>
 </file>
 
@@ -12399,6 +12888,508 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="340">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -12426,6 +13417,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12709,10 +13730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R631"/>
+  <dimension ref="B1:W631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R12" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="T4" workbookViewId="0">
+      <selection activeCell="X72" sqref="X72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13806,7 +14827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>29</v>
       </c>
@@ -13838,7 +14859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>30</v>
       </c>
@@ -13870,7 +14891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>31</v>
       </c>
@@ -13902,7 +14923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>32</v>
       </c>
@@ -13934,7 +14955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>33</v>
       </c>
@@ -13966,7 +14987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>34</v>
       </c>
@@ -13998,7 +15019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>35</v>
       </c>
@@ -14030,7 +15051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>36</v>
       </c>
@@ -14062,7 +15083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>37</v>
       </c>
@@ -14094,7 +15115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>38</v>
       </c>
@@ -14125,8 +15146,17 @@
       <c r="R42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="U42" t="s">
+        <v>5</v>
+      </c>
+      <c r="V42" t="s">
+        <v>3</v>
+      </c>
+      <c r="W42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>39</v>
       </c>
@@ -14157,8 +15187,23 @@
       <c r="R43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="T43" t="s">
+        <v>7</v>
+      </c>
+      <c r="U43">
+        <f>D631</f>
+        <v>2.2704154968261614E-3</v>
+      </c>
+      <c r="V43">
+        <f>H195</f>
+        <v>8.277960429116718E-2</v>
+      </c>
+      <c r="W43">
+        <f>L22</f>
+        <v>6.1884522438037499E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>40</v>
       </c>
@@ -14190,7 +15235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>41</v>
       </c>
@@ -14222,7 +15267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>42</v>
       </c>
@@ -14254,7 +15299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>43</v>
       </c>
@@ -14286,7 +15331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>44</v>
       </c>
@@ -28992,7 +30037,7 @@
     </row>
     <row r="630" spans="2:18" x14ac:dyDescent="0.2">
       <c r="O630">
-        <v>656</v>
+        <v>626</v>
       </c>
       <c r="P630">
         <v>4</v>

</xml_diff>